<commit_message>
pre-release 3 (not fully tested but working yay)
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -307,7 +307,7 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:gapWidth val="50"/>
+        <c:gapWidth val="30"/>
         <c:overlap val="100"/>
         <c:axId val="50010001"/>
         <c:axId val="50010002"/>
@@ -418,7 +418,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" baseline="0">
+              <a:defRPr sz="1000" b="0" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="F0F0F0"/>
                 </a:solidFill>
@@ -488,7 +488,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>

</xml_diff>